<commit_message>
[doc] Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73FF911-067E-4BFC-BA89-BAF440A0E7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265C2CE-FCC3-48D0-AC36-995952D1FFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Auteur:</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Ecriture de l'analyse préliminaire</t>
+  </si>
+  <si>
+    <t>Ecriture de la politique de test</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1101,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4136,7 +4139,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4191,7 +4194,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 5 minutes</v>
+        <v>1 heures 15 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4210,11 +4213,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4298,15 +4301,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="str">
+      <c r="A9" s="74">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B9" s="40">
+        <v>45614</v>
+      </c>
       <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="28"/>
+      <c r="D9" s="42">
+        <v>10</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>33</v>
+      </c>
       <c r="G9" s="46"/>
       <c r="M9" t="s">
         <v>19</v>
@@ -10899,11 +10910,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10911,7 +10922,7 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 05 min</v>
+        <v>1 h 15 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
@@ -10936,22 +10947,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 05 min</v>
+        <v>1 h 15 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>1.231060606060606E-2</v>
+        <v>1.4204545454545454E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -10995,26 +11006,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11237,32 +11228,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11279,4 +11265,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] Updates journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265C2CE-FCC3-48D0-AC36-995952D1FFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E127BE-2E65-4B45-9D10-2B355AE518D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Auteur:</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Ecriture de la politique de test</t>
+  </si>
+  <si>
+    <t>Ecriture de la stratégie de test</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1104,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4194,7 +4197,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 15 minutes</v>
+        <v>1 heures 35 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4213,11 +4216,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4330,15 +4333,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="str">
+      <c r="A10" s="73">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="36"/>
+        <v>47</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45614</v>
+      </c>
       <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="28"/>
+      <c r="D10" s="38">
+        <v>20</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="G10" s="45"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -10910,11 +10921,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10922,7 +10933,7 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 15 min</v>
+        <v>1 h 35 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
@@ -10947,22 +10958,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 15 min</v>
+        <v>1 h 35 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>1.4204545454545454E-2</v>
+        <v>1.7992424242424244E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11006,6 +11017,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11228,27 +11259,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11265,29 +11301,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (plan de test): Ajout du plan de test de l'authentification
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E127BE-2E65-4B45-9D10-2B355AE518D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECDCE74-2A13-4B89-8101-F583FAD85831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -4142,7 +4142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11017,26 +11017,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11259,32 +11239,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11301,4 +11276,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail test): Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECDCE74-2A13-4B89-8101-F583FAD85831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBFC1E9-15A3-4633-AED8-3DE51E6A9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Auteur:</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Ecriture de la stratégie de test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecriture du plan de test de connexion </t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4142,7 +4145,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4200,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 35 minutes</v>
+        <v>1 heures 50 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4216,11 +4219,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4362,15 +4365,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45628</v>
+      </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
+      <c r="D11" s="42">
+        <v>15</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -10921,11 +10932,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10933,7 +10944,7 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 35 min</v>
+        <v>1 h 50 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
@@ -10958,22 +10969,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 35 min</v>
+        <v>1 h 50 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>1.7992424242424244E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11017,6 +11028,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11239,27 +11270,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11276,29 +11312,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (plan de test): Update journal de travail test
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBFC1E9-15A3-4633-AED8-3DE51E6A9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCAE0A8-A80F-4A41-AEAB-FA17D46AA8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Auteur:</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ecriture du plan de test de connexion </t>
+  </si>
+  <si>
+    <t>Vérification + correction des plan de test</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4145,7 +4148,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4200,7 +4203,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 50 minutes</v>
+        <v>2 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4219,11 +4222,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4394,15 +4397,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45628</v>
+      </c>
       <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
+      <c r="D12" s="38">
+        <v>10</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G12" s="45"/>
       <c r="N12">
         <v>5</v>
@@ -10932,11 +10943,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10944,7 +10955,7 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 50 min</v>
+        <v>2 h 00 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
@@ -10969,22 +10980,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 50 min</v>
+        <v>2 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>2.0833333333333332E-2</v>
+        <v>2.2727272727272728E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11028,26 +11039,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11270,32 +11261,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11312,4 +11298,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail test): Update journal de travail test
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A56A652-8AE5-49D3-91AE-D181563A775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF548F1-B366-4395-A3B8-CE224B98E0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Test login (marche pas)</t>
+  </si>
+  <si>
+    <t>Mise en place du test login (création d'un compte)</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1959,13 +1962,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44186046511627908</c:v>
+                  <c:v>0.48936170212765956</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55813953488372092</c:v>
+                  <c:v>0.51063829787234039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4151,7 +4154,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4206,7 +4209,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 35 minutes</v>
+        <v>3 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4225,11 +4228,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4454,15 +4457,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
+        <v>50</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45635</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="38">
+        <v>20</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -10882,11 +10893,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10894,11 +10905,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 35 min</v>
+        <v>1 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.44186046511627908</v>
+        <v>0.48936170212765956</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10972,7 +10983,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.55813953488372092</v>
+        <v>0.51063829787234039</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10993,22 +11004,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 35 min</v>
+        <v>3 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>4.0719696969696968E-2</v>
+        <v>4.450757575757576E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11052,26 +11063,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11294,32 +11285,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11336,4 +11322,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travil) Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B067CFB-C377-49A3-9A4F-5BA27DCC08B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F06E02-FB28-43D5-90CC-DCB347A085CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Auteur:</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Aide philippe</t>
+  </si>
+  <si>
+    <t>Absence</t>
+  </si>
+  <si>
+    <t>Evaluation 80% avec la prof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place des test de gestion de l'utilisateur </t>
   </si>
 </sst>
 </file>
@@ -1116,16 +1125,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>255</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1968,16 +1977,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>2.9197080291970802E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.68</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.68613138686131392</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32</c:v>
+                  <c:v>0.28467153284671531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4163,7 +4172,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4218,7 +4227,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 15 minutes</v>
+        <v>14 heures 25 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4233,15 +4242,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>255</v>
+        <v>385</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>375</v>
+        <v>865</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4334,7 +4343,7 @@
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="42">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>4</v>
@@ -4363,7 +4372,7 @@
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>4</v>
@@ -4385,20 +4394,18 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v>49</v>
-      </c>
-      <c r="B11" s="40">
-        <v>45628</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42">
-        <v>15</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>4</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B11" s="36">
+        <v>45621</v>
+      </c>
+      <c r="C11" s="37">
+        <v>3</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="28" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
@@ -4416,18 +4423,18 @@
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
         <v>49</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="40">
         <v>45628</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38">
-        <v>10</v>
-      </c>
-      <c r="E12" s="39" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="42">
+        <v>40</v>
+      </c>
+      <c r="E12" s="43" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="45"/>
       <c r="N12">
@@ -4442,20 +4449,18 @@
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
         <v>49</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="36">
         <v>45628</v>
       </c>
-      <c r="C13" s="41">
-        <v>1</v>
-      </c>
-      <c r="D13" s="42">
-        <v>35</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>19</v>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38">
+        <v>10</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>4</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="46"/>
       <c r="N13">
@@ -4468,20 +4473,22 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v>50</v>
-      </c>
-      <c r="B14" s="36">
-        <v>45635</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38">
-        <v>20</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>19</v>
+        <v>49</v>
+      </c>
+      <c r="B14" s="40">
+        <v>45628</v>
+      </c>
+      <c r="C14" s="41">
+        <v>1</v>
+      </c>
+      <c r="D14" s="42">
+        <v>35</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>3</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="45"/>
       <c r="N14">
@@ -4496,18 +4503,20 @@
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
         <v>50</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="36">
         <v>45635</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42">
+      <c r="C15" s="37">
+        <v>1</v>
+      </c>
+      <c r="D15" s="38">
         <v>20</v>
       </c>
-      <c r="E15" s="43" t="s">
-        <v>19</v>
+      <c r="E15" s="39" t="s">
+        <v>3</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="46"/>
       <c r="N15">
@@ -4522,20 +4531,20 @@
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
         <v>50</v>
       </c>
-      <c r="B16" s="36">
-        <v>45639</v>
-      </c>
-      <c r="C16" s="37">
+      <c r="B16" s="40">
+        <v>45635</v>
+      </c>
+      <c r="C16" s="41">
         <v>1</v>
       </c>
-      <c r="D16" s="38">
-        <v>30</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>19</v>
+      <c r="D16" s="42">
+        <v>20</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>3</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="45"/>
       <c r="O16">
@@ -4547,18 +4556,20 @@
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
         <v>50</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="36">
         <v>45639</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42">
+      <c r="C17" s="37">
+        <v>1</v>
+      </c>
+      <c r="D17" s="38">
         <v>30</v>
       </c>
-      <c r="E17" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="80" t="s">
-        <v>41</v>
+      <c r="E17" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="G17" s="46"/>
       <c r="O17">
@@ -4566,45 +4577,71 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="str">
+      <c r="A18" s="73">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="B18" s="40">
+        <v>45639</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42">
+        <v>45</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="80" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" s="45"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="str">
+      <c r="A19" s="74">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="B19" s="36">
+        <v>45642</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38">
+        <v>20</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>43</v>
+      </c>
       <c r="G19" s="46"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="str">
+      <c r="A20" s="73">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="B20" s="36">
+        <v>45642</v>
+      </c>
+      <c r="C20" s="37">
+        <v>1</v>
+      </c>
+      <c r="D20" s="38">
+        <v>20</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -10891,11 +10928,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10903,11 +10940,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 20 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0</v>
+        <v>2.9197080291970802E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10924,15 +10961,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10940,11 +10977,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 15 min</v>
+        <v>0 h 00 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10961,15 +10998,15 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="E8" s="22" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10977,11 +11014,11 @@
       </c>
       <c r="F8" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>7 h 50 min</v>
       </c>
       <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.68613138686131392</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11002,11 +11039,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11014,11 +11051,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 00 min</v>
+        <v>3 h 15 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.32</v>
+        <v>0.28467153284671531</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11035,26 +11072,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>255</v>
+        <v>385</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>375</v>
+        <v>685</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 15 min</v>
+        <v>11 h 25 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>7.1022727272727279E-2</v>
+        <v>0.12973484848484848</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11098,6 +11135,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11320,15 +11366,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11341,6 +11378,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11355,14 +11400,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[doc] (journal de travail ) Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26A55AE-072D-41FE-9AD4-315F870CF793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D57982E-7522-47A1-B0A4-AA76F8C3804A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Auteur:</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Mise en place d'un test unitaire pour la création d'une todo</t>
+  </si>
+  <si>
+    <t>Mise en place d'un test unitaire pour la suppréssion d'une todo d'une todo</t>
+  </si>
+  <si>
+    <t>Mise en place d'un test unitaire pour la modification d'une todo d'une todo</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1140,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>195</c:v>
@@ -1980,16 +1986,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.8368794326241134E-2</c:v>
+                  <c:v>2.7027027027027029E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69503546099290781</c:v>
+                  <c:v>0.70945945945945943</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27659574468085107</c:v>
+                  <c:v>0.26351351351351349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4175,7 +4181,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4230,7 +4236,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>14 heures 45 minutes</v>
+        <v>15 heures 20 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4249,11 +4255,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>885</v>
+        <v>920</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4668,27 +4674,43 @@
       <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="str">
+      <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="B22" s="36">
+        <v>45642</v>
+      </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
+      <c r="D22" s="38">
+        <v>30</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="74">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B23" s="40">
+        <v>45642</v>
+      </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
+      <c r="D23" s="42">
+        <v>5</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>47</v>
+      </c>
       <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -10955,7 +10977,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11013,11 +11035,11 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>490</v>
+        <v>525</v>
       </c>
       <c r="E8" s="22" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11025,11 +11047,11 @@
       </c>
       <c r="F8" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 10 min</v>
+        <v>8 h 45 min</v>
       </c>
       <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>0.69503546099290781</v>
+        <v>0.70945945945945943</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11066,7 +11088,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.27659574468085107</v>
+        <v>0.26351351351351349</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11087,22 +11109,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>705</v>
+        <v>740</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 45 min</v>
+        <v>12 h 20 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.13352272727272727</v>
+        <v>0.14015151515151514</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>